<commit_message>
JW and LvdB: modifying excel file on crops energy content
</commit_message>
<xml_diff>
--- a/Crops energy content.xlsx
+++ b/Crops energy content.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\新建文件夹\新建文件夹\Questionnaire\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\OneDrive\Documenten\ACT - personal\Project\LCA analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587E6C96-AB7D-4D55-AE31-37E8F146B19C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{587E6C96-AB7D-4D55-AE31-37E8F146B19C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{B5DF5F86-C59E-4B34-A53A-E700DC9269E7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Basic database" sheetId="2" r:id="rId1"/>
+    <sheet name="Expanded database" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="62">
   <si>
     <t>NEVO-code</t>
   </si>
@@ -220,13 +221,16 @@
   <si>
     <t>Lettuce</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Microgreen mix AH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -281,7 +285,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -297,7 +301,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -592,26 +596,406 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B15C82-8EF1-4B9A-8A3F-DA9A7F99F0F7}">
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1">
+        <v>1399</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="1">
+        <v>62</v>
+      </c>
+      <c r="E2" s="1">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>95.7</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1">
+        <v>71</v>
+      </c>
+      <c r="E3" s="1">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>95.3</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1">
+        <v>51</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="1">
+        <v>108</v>
+      </c>
+      <c r="E4" s="1">
+        <v>26</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>91.9</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="1">
+        <v>58</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="1">
+        <v>97</v>
+      </c>
+      <c r="E5" s="1">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>93</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="1">
+        <v>128</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="1">
+        <v>125</v>
+      </c>
+      <c r="E6" s="1">
+        <v>30</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>5</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>87</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="1">
+        <v>959</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="1">
+        <v>193</v>
+      </c>
+      <c r="E7" s="1">
+        <v>46</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>86</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="1">
+        <v>2177</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1">
+        <v>200</v>
+      </c>
+      <c r="E8" s="1">
+        <v>48</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="I8" s="1">
+        <v>3.9</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="1">
+        <v>2736</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="1">
+        <v>98</v>
+      </c>
+      <c r="E9" s="1">
+        <v>23</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>87</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="C10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="1">
+        <v>32</v>
+      </c>
+      <c r="K10" s="1">
+        <v>96.7</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:M44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="3" max="3" width="14.42578125" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -642,7 +1026,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="12.75">
       <c r="A2" s="1">
         <v>1399</v>
       </c>
@@ -680,14 +1064,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="12.75">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="1">
@@ -718,14 +1102,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="12.75">
       <c r="A4" s="1">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="1">
@@ -756,14 +1140,14 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="12.75">
       <c r="A5" s="1">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="1">
@@ -794,14 +1178,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="12.75">
       <c r="A6" s="1">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="1">
@@ -832,14 +1216,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="12.75">
       <c r="A7" s="1">
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="1">
@@ -870,7 +1254,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="12.75">
       <c r="A8" s="1">
         <v>41</v>
       </c>
@@ -908,7 +1292,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="12.75">
       <c r="A9" s="1">
         <v>51</v>
       </c>
@@ -946,7 +1330,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="12.75">
       <c r="A10" s="1">
         <v>58</v>
       </c>
@@ -984,7 +1368,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="12.75">
       <c r="A11" s="1">
         <v>60</v>
       </c>
@@ -1022,7 +1406,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="12.75">
       <c r="A12" s="1">
         <v>63</v>
       </c>
@@ -1060,7 +1444,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="12.75">
       <c r="A13" s="1">
         <v>67</v>
       </c>
@@ -1098,7 +1482,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="12.75">
       <c r="A14" s="1">
         <v>71</v>
       </c>
@@ -1136,7 +1520,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="12.75">
       <c r="A15" s="1">
         <v>128</v>
       </c>
@@ -1174,7 +1558,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="12.75">
       <c r="A16" s="1">
         <v>562</v>
       </c>
@@ -1212,7 +1596,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="12.75">
       <c r="A17" s="1">
         <v>829</v>
       </c>
@@ -1250,7 +1634,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="12.75">
       <c r="A18" s="1">
         <v>884</v>
       </c>
@@ -1288,7 +1672,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="12.75">
       <c r="A19" s="1">
         <v>921</v>
       </c>
@@ -1326,7 +1710,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="12.75">
       <c r="A20" s="1">
         <v>922</v>
       </c>
@@ -1364,7 +1748,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="12.75">
       <c r="A21" s="1">
         <v>959</v>
       </c>
@@ -1402,14 +1786,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1">
       <c r="A22" s="1">
         <v>2177</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D22" s="1">
@@ -1434,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="12.75">
       <c r="A23" s="1">
         <v>2736</v>
       </c>
@@ -1472,7 +1856,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="12.75">
       <c r="A24" s="1">
         <v>2739</v>
       </c>
@@ -1510,8 +1894,8 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="C25" s="1" t="s">
+    <row r="25" spans="1:12" ht="12.75">
+      <c r="C25" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E25" s="1">
@@ -1524,7 +1908,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="15.75" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>43</v>
       </c>

</xml_diff>